<commit_message>
Added changes for the error message.
More detailed error message used for data validation.
</commit_message>
<xml_diff>
--- a/Arc5Rewards.xlsx
+++ b/Arc5Rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://panduit-my.sharepoint.com/personal/chsh_panduit_com/Documents/Documents/Personnel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{12A1EFEE-C1B1-4271-BB89-8593FE2713C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{11986487-6749-4550-92B4-5A24DAB65C6B}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="8_{12A1EFEE-C1B1-4271-BB89-8593FE2713C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{31AAEDED-D1E6-4FE2-B083-03A2DADC962C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{108CB1B5-0773-4018-BEC9-941D178DECF2}"/>
   </bookViews>
@@ -330,24 +330,24 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -400,51 +400,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFCDCD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -460,51 +420,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FFC00000"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFCDCD"/>
         </patternFill>
       </fill>
     </dxf>
@@ -515,226 +435,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCDCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1066,8 +766,8 @@
   <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1077,8 +777,8 @@
     <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
@@ -1093,7 +793,7 @@
       <c r="A2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <f>SUM(H5:H68)</f>
         <v>0</v>
       </c>
@@ -1112,21 +812,21 @@
       <c r="F3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="8" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D5" s="5" t="s">
@@ -1136,8 +836,8 @@
       <c r="F5" s="5">
         <v>6000</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9">
         <f>F5*G5</f>
         <v>0</v>
       </c>
@@ -1150,8 +850,8 @@
       <c r="F6" s="5">
         <v>6000</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9">
         <f t="shared" ref="H6:H68" si="0">F6*G6</f>
         <v>0</v>
       </c>
@@ -1164,8 +864,8 @@
       <c r="F7" s="5">
         <v>2000</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1178,8 +878,8 @@
       <c r="F8" s="5">
         <v>7000</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1192,8 +892,8 @@
       <c r="F9" s="5">
         <v>2000</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1206,8 +906,8 @@
       <c r="F10" s="5">
         <v>6000</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1220,8 +920,8 @@
       <c r="F11" s="5">
         <v>6000</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1234,20 +934,20 @@
       <c r="F12" s="5">
         <v>2000</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D14" s="5" t="s">
@@ -1257,8 +957,8 @@
       <c r="F14" s="5">
         <v>3000</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1271,8 +971,8 @@
       <c r="F15" s="5">
         <v>3000</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11">
+      <c r="G15" s="9"/>
+      <c r="H15" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1285,8 +985,8 @@
       <c r="F16" s="5">
         <v>3750</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1299,20 +999,20 @@
       <c r="F17" s="5">
         <v>2500</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11">
+      <c r="G17" s="9"/>
+      <c r="H17" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D19" s="5" t="s">
@@ -1324,8 +1024,8 @@
       <c r="F19" s="5">
         <v>21200</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1340,8 +1040,8 @@
       <c r="F20" s="5">
         <v>21200</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11">
+      <c r="G20" s="9"/>
+      <c r="H20" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1356,8 +1056,8 @@
       <c r="F21" s="5">
         <v>21200</v>
       </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11">
+      <c r="G21" s="9"/>
+      <c r="H21" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1372,8 +1072,8 @@
       <c r="F22" s="5">
         <v>8800</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11">
+      <c r="G22" s="9"/>
+      <c r="H22" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1388,8 +1088,8 @@
       <c r="F23" s="5">
         <v>8800</v>
       </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11">
+      <c r="G23" s="9"/>
+      <c r="H23" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1404,8 +1104,8 @@
       <c r="F24" s="5">
         <v>8800</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11">
+      <c r="G24" s="9"/>
+      <c r="H24" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1420,8 +1120,8 @@
       <c r="F25" s="5">
         <v>2600</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11">
+      <c r="G25" s="9"/>
+      <c r="H25" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1436,8 +1136,8 @@
       <c r="F26" s="5">
         <v>2600</v>
       </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11">
+      <c r="G26" s="9"/>
+      <c r="H26" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1452,8 +1152,8 @@
       <c r="F27" s="5">
         <v>2600</v>
       </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11">
+      <c r="G27" s="9"/>
+      <c r="H27" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1468,8 +1168,8 @@
       <c r="F28" s="5">
         <v>1500</v>
       </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11">
+      <c r="G28" s="9"/>
+      <c r="H28" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1482,8 +1182,8 @@
       <c r="F29" s="5">
         <v>3800</v>
       </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11">
+      <c r="G29" s="9"/>
+      <c r="H29" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1498,8 +1198,8 @@
       <c r="F30" s="5">
         <v>300</v>
       </c>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11">
+      <c r="G30" s="9"/>
+      <c r="H30" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1514,8 +1214,8 @@
       <c r="F31" s="5">
         <v>400</v>
       </c>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11">
+      <c r="G31" s="9"/>
+      <c r="H31" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1530,8 +1230,8 @@
       <c r="F32" s="5">
         <v>3800</v>
       </c>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11">
+      <c r="G32" s="9"/>
+      <c r="H32" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1546,8 +1246,8 @@
       <c r="F33" s="5">
         <v>3800</v>
       </c>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11">
+      <c r="G33" s="9"/>
+      <c r="H33" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1562,20 +1262,20 @@
       <c r="F34" s="5">
         <v>1200</v>
       </c>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11">
+      <c r="G34" s="9"/>
+      <c r="H34" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="4:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
     </row>
     <row r="36" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D36" s="5" t="s">
@@ -1585,8 +1285,8 @@
       <c r="F36" s="5">
         <v>1900</v>
       </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11">
+      <c r="G36" s="9"/>
+      <c r="H36" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1599,8 +1299,8 @@
       <c r="F37" s="5">
         <v>1900</v>
       </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11">
+      <c r="G37" s="9"/>
+      <c r="H37" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1613,8 +1313,8 @@
       <c r="F38" s="5">
         <v>1900</v>
       </c>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11">
+      <c r="G38" s="9"/>
+      <c r="H38" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1627,8 +1327,8 @@
       <c r="F39" s="5">
         <v>2800</v>
       </c>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11">
+      <c r="G39" s="9"/>
+      <c r="H39" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1641,8 +1341,8 @@
       <c r="F40" s="5">
         <v>2800</v>
       </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11">
+      <c r="G40" s="9"/>
+      <c r="H40" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1655,8 +1355,8 @@
       <c r="F41" s="5">
         <v>2800</v>
       </c>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11">
+      <c r="G41" s="9"/>
+      <c r="H41" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1671,8 +1371,8 @@
       <c r="F42" s="5">
         <v>75000</v>
       </c>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11">
+      <c r="G42" s="9"/>
+      <c r="H42" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1685,8 +1385,8 @@
       <c r="F43" s="5">
         <v>1000</v>
       </c>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11">
+      <c r="G43" s="9"/>
+      <c r="H43" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1699,8 +1399,8 @@
       <c r="F44" s="5">
         <v>1100</v>
       </c>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11">
+      <c r="G44" s="9"/>
+      <c r="H44" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1715,8 +1415,8 @@
       <c r="F45" s="5">
         <v>5900</v>
       </c>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11">
+      <c r="G45" s="9"/>
+      <c r="H45" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1729,8 +1429,8 @@
       <c r="F46" s="5">
         <v>30000</v>
       </c>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11">
+      <c r="G46" s="9"/>
+      <c r="H46" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1743,8 +1443,8 @@
       <c r="F47" s="5">
         <v>75000</v>
       </c>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11">
+      <c r="G47" s="9"/>
+      <c r="H47" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1757,8 +1457,8 @@
       <c r="F48" s="5">
         <v>75000</v>
       </c>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11">
+      <c r="G48" s="9"/>
+      <c r="H48" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1771,8 +1471,8 @@
       <c r="F49" s="5">
         <v>75000</v>
       </c>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11">
+      <c r="G49" s="9"/>
+      <c r="H49" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1785,8 +1485,8 @@
       <c r="F50" s="5">
         <v>2900</v>
       </c>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11">
+      <c r="G50" s="9"/>
+      <c r="H50" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1801,8 +1501,8 @@
       <c r="F51" s="5">
         <v>18800</v>
       </c>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11">
+      <c r="G51" s="9"/>
+      <c r="H51" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1815,8 +1515,8 @@
       <c r="F52" s="5">
         <v>1500</v>
       </c>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11">
+      <c r="G52" s="9"/>
+      <c r="H52" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1829,8 +1529,8 @@
       <c r="F53" s="5">
         <v>900</v>
       </c>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11">
+      <c r="G53" s="9"/>
+      <c r="H53" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1843,20 +1543,20 @@
       <c r="F54" s="5">
         <v>1100</v>
       </c>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11">
+      <c r="G54" s="9"/>
+      <c r="H54" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="4:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
     </row>
     <row r="56" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D56" s="5" t="s">
@@ -1868,8 +1568,8 @@
       <c r="F56" s="5">
         <v>450000</v>
       </c>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11">
+      <c r="G56" s="9"/>
+      <c r="H56" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1884,8 +1584,8 @@
       <c r="F57" s="5">
         <v>450000</v>
       </c>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11">
+      <c r="G57" s="9"/>
+      <c r="H57" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1900,8 +1600,8 @@
       <c r="F58" s="5">
         <v>75000</v>
       </c>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11">
+      <c r="G58" s="9"/>
+      <c r="H58" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1916,8 +1616,8 @@
       <c r="F59" s="5">
         <v>150000</v>
       </c>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11">
+      <c r="G59" s="9"/>
+      <c r="H59" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1932,8 +1632,8 @@
       <c r="F60" s="5">
         <v>150000</v>
       </c>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11">
+      <c r="G60" s="9"/>
+      <c r="H60" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1948,8 +1648,8 @@
       <c r="F61" s="5">
         <v>450000</v>
       </c>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11">
+      <c r="G61" s="9"/>
+      <c r="H61" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1964,8 +1664,8 @@
       <c r="F62" s="5">
         <v>450000</v>
       </c>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11">
+      <c r="G62" s="9"/>
+      <c r="H62" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1980,8 +1680,8 @@
       <c r="F63" s="5">
         <v>150000</v>
       </c>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11">
+      <c r="G63" s="9"/>
+      <c r="H63" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1996,8 +1696,8 @@
       <c r="F64" s="5">
         <v>450000</v>
       </c>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11">
+      <c r="G64" s="9"/>
+      <c r="H64" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2012,8 +1712,8 @@
       <c r="F65" s="5">
         <v>450000</v>
       </c>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11">
+      <c r="G65" s="9"/>
+      <c r="H65" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2028,8 +1728,8 @@
       <c r="F66" s="5">
         <v>150000</v>
       </c>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11">
+      <c r="G66" s="9"/>
+      <c r="H66" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2044,8 +1744,8 @@
       <c r="F67" s="5">
         <v>450000</v>
       </c>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11">
+      <c r="G67" s="9"/>
+      <c r="H67" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2060,8 +1760,8 @@
       <c r="F68" s="5">
         <v>450000</v>
       </c>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11">
+      <c r="G68" s="9"/>
+      <c r="H68" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2075,13 +1775,13 @@
     <mergeCell ref="D55:H55"/>
   </mergeCells>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G12">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>IF(ISNUMBER(E7),IF(G7&gt;E7,TRUE,FALSE),FALSE)</formula>
+  <conditionalFormatting sqref="G19:G34">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+      <formula>IF(ISNUMBER(E19),IF(G19&gt;E19,TRUE,FALSE),FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14:G17">
@@ -2089,9 +1789,9 @@
       <formula>IF(ISNUMBER(E14),IF(G14&gt;E14,TRUE,FALSE),FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G19:G34">
+  <conditionalFormatting sqref="G5:G12">
     <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>IF(ISNUMBER(E19),IF(G19&gt;E19,TRUE,FALSE),FALSE)</formula>
+      <formula>IF(ISNUMBER(E5),IF(G5&gt;E5,TRUE,FALSE),FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36:G54">
@@ -2105,7 +1805,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Don't use Scopley Math" error="Scopely math is not allowed at this level." sqref="G36:G54 G19:G34 G14:G17 G5:G12 G56:G68" xr:uid="{4AD1EDAD-D5E0-441B-B190-C88784A60F92}">
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Don't use Bad Math" error="Bad math is not allowed at this level." sqref="G19:G34 G14:G17 G5:G12 G36:G54 G56:G68" xr:uid="{750B6DF3-8879-4788-9F98-3449B7D82E19}">
       <formula1>0</formula1>
       <formula2>E5</formula2>
     </dataValidation>

</xml_diff>